<commit_message>
Updating Food Diary.xlxs; removing other sheets
</commit_message>
<xml_diff>
--- a/Food Diary.xlsx
+++ b/Food Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\Box\TC\Personal\Food\Food\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB61A62-52AA-4873-8D8F-5FED4926662A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DCDD9D-0FB6-45EB-BC1C-0529CCD97870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="22776" windowHeight="13176" xr2:uid="{05A5D1BC-1B43-42BE-9C8B-CDB5140BAB23}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -667,8 +667,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3399,6 +3399,12 @@
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>44269</v>
+      </c>
+      <c r="B247" t="s">
+        <v>15</v>
+      </c>
+      <c r="C247">
+        <v>23</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>